<commit_message>
ct4 and ct6 fix
</commit_message>
<xml_diff>
--- a/UZ-REPOS/SPA/EDITION/DOC/ALLPLAY/Модель услуг CT6.xlsx
+++ b/UZ-REPOS/SPA/EDITION/DOC/ALLPLAY/Модель услуг CT6.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Версия</t>
   </si>
@@ -42,9 +42,6 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>Черкашин К.Л.</t>
-  </si>
-  <si>
     <t>Первая версия модели услуг</t>
   </si>
   <si>
@@ -136,6 +133,18 @@
   </si>
   <si>
     <t>Мобильное ТВ 7 дней</t>
+  </si>
+  <si>
+    <t>Ресурс</t>
+  </si>
+  <si>
+    <t>Хованский В.Д.</t>
+  </si>
+  <si>
+    <t>RES_CT6_SERVICE_ID</t>
+  </si>
+  <si>
+    <t>mobtv</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
     <numFmt numFmtId="164" formatCode="[$-419]General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$руб.-419];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$руб.-419]"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +261,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,8 +311,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -409,22 +430,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -433,15 +439,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -461,21 +458,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -552,22 +534,79 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
@@ -579,8 +618,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -616,9 +656,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,49 +671,31 @@
     <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -685,18 +704,46 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Heading" xfId="2"/>
     <cellStyle name="Heading1" xfId="3"/>
+    <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="4"/>
     <cellStyle name="Result2" xfId="5"/>
@@ -980,7 +1027,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,14 +1069,14 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1054,15 +1101,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5"/>
     </row>
@@ -1095,62 +1142,62 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="10" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>18</v>
-      </c>
       <c r="B4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="10" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1169,130 +1216,141 @@
   <dimension ref="A1:AMN58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="17.75" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19" style="15" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="15" customWidth="1"/>
-    <col min="5" max="5" width="17.875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="27.375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="9.875" style="15" customWidth="1"/>
-    <col min="8" max="8" width="28.125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="15" customWidth="1"/>
-    <col min="10" max="10" width="14.125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="13" style="15" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="15" customWidth="1"/>
-    <col min="13" max="13" width="11.875" style="15" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="15" customWidth="1"/>
-    <col min="15" max="15" width="18.625" style="15" customWidth="1"/>
-    <col min="16" max="16" width="46.625" style="14" customWidth="1"/>
-    <col min="17" max="1028" width="8.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="13.375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="14" customWidth="1"/>
+    <col min="3" max="3" width="19" style="14" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="27.375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="9.875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="28.125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="9.875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="13" style="14" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="14" customWidth="1"/>
+    <col min="13" max="13" width="11.875" style="14" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="14" customWidth="1"/>
+    <col min="15" max="15" width="18.625" style="14" customWidth="1"/>
+    <col min="16" max="16" width="46.625" style="13" customWidth="1"/>
+    <col min="17" max="1028" width="8.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="B2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F3" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="E4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="30"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1321,412 +1379,412 @@
     <row r="33" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="13"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>